<commit_message>
Updated analyzer logic and config
</commit_message>
<xml_diff>
--- a/what_test_controls.xlsx
+++ b/what_test_controls.xlsx
@@ -1,33 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/final_consolidated_analyzer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_B0DEFEC297D9AECF8A160B365BCB643B55D8FDCE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F69C06D8-43BF-4E8A-88FD-9DF224FCC3A9}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
-    <t>Control_ID</t>
-  </si>
-  <si>
-    <t>Control_Description</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
-    <t>Control_Type</t>
-  </si>
-  <si>
     <t>CTRL-001</t>
   </si>
   <si>
@@ -134,13 +131,22 @@
   </si>
   <si>
     <t>Preventive</t>
+  </si>
+  <si>
+    <t>Control ID</t>
+  </si>
+  <si>
+    <t>Control Description</t>
+  </si>
+  <si>
+    <t>Control Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,13 +209,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +261,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -281,6 +295,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -315,9 +330,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,235 +506,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>